<commit_message>
new classes added : excelutil and screenshot login and checkout functionality
</commit_message>
<xml_diff>
--- a/MyOGProject/TestData/TestFile.xlsx
+++ b/MyOGProject/TestData/TestFile.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Upgraded_sel\OnlineOliveBooking\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\git\OliveGarden_Framework\MyOGProject\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699B5CAD-22DB-45A5-B815-0F9F5DAAF6F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA95D60-72B9-49D0-9584-F0E9BDAC43C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DD7F6292-3989-4207-B15C-45DEDA918A7D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{DD7F6292-3989-4207-B15C-45DEDA918A7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Email</t>
   </si>
@@ -67,6 +68,39 @@
   </si>
   <si>
     <t>March</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>hitendravibhandik1@gmail.com</t>
+  </si>
+  <si>
+    <t>Hitesh@222</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>Apt no</t>
+  </si>
+  <si>
+    <t>carmel drive</t>
+  </si>
+  <si>
+    <t>A453</t>
+  </si>
+  <si>
+    <t>B305</t>
+  </si>
+  <si>
+    <t>Guests</t>
+  </si>
+  <si>
+    <t>rochester hills</t>
   </si>
 </sst>
 </file>
@@ -111,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -119,6 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -436,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFE452A4-8CB7-4ACB-A090-560DC953351B}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -529,4 +564,80 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE8946F-DB00-4CB9-A791-405185BB80A3}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{2400F8FD-AC34-4FF0-ABC1-174F3FD16074}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0E5AB1FD-4D25-42A5-B9FD-7B677F6B13FA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>